<commit_message>
4 not 3 in spreadsheet
</commit_message>
<xml_diff>
--- a/resources/Tutorial 0 - Spreadsheet Practice.xlsx
+++ b/resources/Tutorial 0 - Spreadsheet Practice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/55130566/Documents/Teaching Content/Maths for Data Science/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/55130566/Documents/Teaching Content/Maths for Data Science/Tutorial Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58E73C23-88FD-D046-B0E9-DD5A1DD6CA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE3055A-F87E-254A-A9CE-78062B07C7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" activeTab="3" xr2:uid="{A829DC27-3655-5B43-950C-310622157006}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{A829DC27-3655-5B43-950C-310622157006}"/>
   </bookViews>
   <sheets>
     <sheet name="Task 1" sheetId="5" r:id="rId1"/>
@@ -693,9 +693,6 @@
     <t>5. Clear your filter, then use the 'Text to columns' tool to make this table have an additional column, which is blank if the Pokemon has only one type, and contains its second type otherwise. Head these columns 'Type 1' and 'Type 2'.</t>
   </si>
   <si>
-    <t>6. Repeat step 3.</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
@@ -955,6 +952,9 @@
   </si>
   <si>
     <t>Enter formulae in the cells highlighted yellow to complete the tables. Click on the blue cells to see a hint in the formula bar, if you need one.</t>
+  </si>
+  <si>
+    <t>6. Repeat step 4.</t>
   </si>
 </sst>
 </file>
@@ -962,10 +962,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ am/pm"/>
-    <numFmt numFmtId="173" formatCode="00000"/>
-    <numFmt numFmtId="174" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1167,24 +1167,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1195,46 +1224,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1572,53 +1566,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB1C586-BAC7-1840-8B5C-73B3B3C579E6}">
   <dimension ref="B3:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="98.6640625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="98.6640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="54" customHeight="1">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="61" customHeight="1">
-      <c r="B4" s="5" t="s">
-        <v>224</v>
+      <c r="B4" s="4" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="61" customHeight="1">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="47" customHeight="1">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="106" customHeight="1">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="61" customHeight="1">
-      <c r="B8" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="69">
-      <c r="B9" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="46">
+      <c r="B9" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="46">
+      <c r="B11" s="4" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="46">
-      <c r="B11" s="5" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1636,17 +1632,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="33"/>
-    <col min="2" max="2" width="14.83203125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="69.6640625" style="33" customWidth="1"/>
-    <col min="4" max="5" width="14.33203125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="38" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="39" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="33" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="33"/>
+    <col min="1" max="1" width="10.83203125" style="25"/>
+    <col min="2" max="2" width="14.83203125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="69.6640625" style="25" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="29" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="30" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="25" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" s="33" customFormat="1">
+    <row r="2" spans="2:8">
       <c r="B2" s="2" t="s">
         <v>199</v>
       </c>
@@ -1659,17 +1655,17 @@
       <c r="E2" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="24" t="s">
         <v>203</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="33" customFormat="1">
+    <row r="3" spans="2:8">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -1679,20 +1675,20 @@
       <c r="D3" s="2">
         <v>1994</v>
       </c>
-      <c r="E3" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="35">
+      <c r="E3" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" s="27">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="23" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="33" customFormat="1">
+    <row r="4" spans="2:8">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -1702,20 +1698,20 @@
       <c r="D4" s="2">
         <v>1972</v>
       </c>
-      <c r="E4" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="G4" s="36">
+      <c r="E4" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="23" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="33" customFormat="1">
+    <row r="5" spans="2:8">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -1725,20 +1721,20 @@
       <c r="D5" s="2">
         <v>2008</v>
       </c>
-      <c r="E5" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="G5" s="36">
+      <c r="E5" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="G5" s="2">
         <v>9.1</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="23" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="33" customFormat="1">
+    <row r="6" spans="2:8">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -1748,20 +1744,20 @@
       <c r="D6" s="2">
         <v>1974</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="G6" s="35">
+      <c r="E6" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="G6" s="27">
         <v>9</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="23" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="33" customFormat="1">
+    <row r="7" spans="2:8">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -1771,20 +1767,20 @@
       <c r="D7" s="2">
         <v>1957</v>
       </c>
-      <c r="E7" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="G7" s="35">
+      <c r="E7" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" s="27">
         <v>9</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="23" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="33" customFormat="1">
+    <row r="8" spans="2:8">
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -1794,20 +1790,20 @@
       <c r="D8" s="2">
         <v>2003</v>
       </c>
-      <c r="E8" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="G8" s="35">
+      <c r="E8" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="G8" s="27">
         <v>9</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="23" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="33" customFormat="1">
+    <row r="9" spans="2:8">
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -1817,20 +1813,20 @@
       <c r="D9" s="2">
         <v>1993</v>
       </c>
-      <c r="E9" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="G9" s="35">
+      <c r="E9" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="G9" s="27">
         <v>9</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="33" customFormat="1">
+    <row r="10" spans="2:8">
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -1840,20 +1836,20 @@
       <c r="D10" s="2">
         <v>2001</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="G10" s="36">
+      <c r="E10" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" s="2">
         <v>8.9</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="23" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="33" customFormat="1">
+    <row r="11" spans="2:8">
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -1863,20 +1859,20 @@
       <c r="D11" s="2">
         <v>1994</v>
       </c>
-      <c r="E11" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="G11" s="36">
+      <c r="E11" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" s="2">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="23" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="33" customFormat="1">
+    <row r="12" spans="2:8">
       <c r="B12" s="2">
         <v>10</v>
       </c>
@@ -1886,118 +1882,78 @@
       <c r="D12" s="2">
         <v>1966</v>
       </c>
-      <c r="E12" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="G12" s="36">
+      <c r="E12" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="G12" s="2">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="23" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="33" customFormat="1">
-      <c r="C14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-    </row>
-    <row r="15" spans="2:8" s="33" customFormat="1">
-      <c r="C15" s="40"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-    </row>
-    <row r="18" spans="3:7" s="33" customFormat="1">
-      <c r="C18" s="37"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-    </row>
-    <row r="19" spans="3:7" s="33" customFormat="1">
-      <c r="C19" s="40"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-    </row>
-    <row r="22" spans="3:7" s="33" customFormat="1">
-      <c r="C22" s="37"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-    </row>
-    <row r="23" spans="3:7" s="33" customFormat="1">
-      <c r="C23" s="40"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-    </row>
-    <row r="26" spans="3:7" s="33" customFormat="1">
-      <c r="C26" s="37"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="39"/>
-    </row>
-    <row r="27" spans="3:7" s="33" customFormat="1">
-      <c r="C27" s="40"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="39"/>
-    </row>
-    <row r="30" spans="3:7" s="33" customFormat="1">
-      <c r="C30" s="37"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="39"/>
-    </row>
-    <row r="31" spans="3:7" s="33" customFormat="1">
-      <c r="C31" s="40"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="39"/>
-    </row>
-    <row r="34" spans="3:7" s="33" customFormat="1">
-      <c r="C34" s="37"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="39"/>
-    </row>
-    <row r="35" spans="3:7" s="33" customFormat="1">
-      <c r="C35" s="40"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
-    </row>
-    <row r="38" spans="3:7" s="33" customFormat="1">
-      <c r="C38" s="37"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="39"/>
-    </row>
-    <row r="39" spans="3:7" s="33" customFormat="1">
-      <c r="C39" s="40"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="39"/>
-    </row>
-    <row r="42" spans="3:7" s="33" customFormat="1">
-      <c r="C42" s="37"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="39"/>
-    </row>
-    <row r="43" spans="3:7" s="33" customFormat="1">
-      <c r="C43" s="40"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="39"/>
-    </row>
-    <row r="46" spans="3:7" s="33" customFormat="1">
-      <c r="C46" s="37"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="39"/>
-    </row>
-    <row r="47" spans="3:7" s="33" customFormat="1">
-      <c r="C47" s="40"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="39"/>
-    </row>
-    <row r="50" spans="3:7" s="33" customFormat="1">
-      <c r="C50" s="37"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="39"/>
-    </row>
-    <row r="51" spans="3:7" s="33" customFormat="1">
-      <c r="C51" s="40"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="39"/>
+    <row r="14" spans="2:8">
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="C15" s="31"/>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="28"/>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="31"/>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" s="28"/>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" s="31"/>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" s="28"/>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" s="31"/>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" s="31"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="28"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="31"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="28"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="31"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="28"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="31"/>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="28"/>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="31"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="28"/>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="31"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G55">
@@ -3852,9 +3808,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C64FAA-2A5B-9240-A02E-FD92E3754DCD}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A3:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3870,656 +3826,613 @@
     <col min="17" max="17" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" ht="45" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" ht="21" customHeight="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:17" ht="37" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" ht="19">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10" t="s">
+    <row r="3" spans="1:16" ht="45" customHeight="1">
+      <c r="B3" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" ht="21" customHeight="1">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" ht="37" customHeight="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" ht="19">
+      <c r="A6" s="7"/>
+      <c r="B6" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" ht="19">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="10" t="s">
+      <c r="C7" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8" t="s">
+      <c r="I7" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" ht="19">
+      <c r="A8" s="7"/>
+      <c r="B8" s="10">
+        <v>15131.229278417033</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="11">
+        <v>128.05799999999999</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="J8" s="12">
+        <v>72900</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" ht="19">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10">
+        <v>21689.879773785746</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" s="11">
+        <v>58.407999999999994</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="J9" s="12">
+        <v>13225</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" ht="19">
+      <c r="A10" s="7"/>
+      <c r="B10" s="10">
+        <v>6556.4431594744028</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D10" s="11">
+        <v>79.97399999999999</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="J10" s="12">
+        <v>15870</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" ht="19">
+      <c r="A11" s="7"/>
+      <c r="B11" s="10">
+        <v>18937.566436409343</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" s="11">
+        <v>479.988</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="J11" s="12">
+        <v>12321</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:16" ht="19">
+      <c r="A12" s="7"/>
+      <c r="B12" s="10">
+        <v>18446.91754397425</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="11">
+        <v>11.808</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" ht="19">
-      <c r="A7" s="8"/>
-      <c r="B7" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:17" ht="19">
-      <c r="A8" s="8"/>
-      <c r="B8" s="15">
-        <v>15131.229278417033</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="I12" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="J12" s="16">
+        <v>25921</v>
+      </c>
+      <c r="K12" s="17"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" ht="19">
+      <c r="A13" s="7"/>
+      <c r="B13" s="10">
+        <v>22337.723635387698</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D8" s="16">
-        <v>128.05799999999999</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="J8" s="17">
-        <v>72900</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" spans="1:17" ht="19">
-      <c r="A9" s="8"/>
-      <c r="B9" s="15">
-        <v>21689.879773785746</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D9" s="16">
-        <v>58.407999999999994</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="J9" s="17">
-        <v>13225</v>
-      </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" ht="19">
-      <c r="A10" s="8"/>
-      <c r="B10" s="15">
-        <v>6556.4431594744028</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D10" s="16">
-        <v>79.97399999999999</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="J10" s="17">
-        <v>15870</v>
-      </c>
-      <c r="K10" s="18"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" ht="19">
-      <c r="A11" s="8"/>
-      <c r="B11" s="15">
-        <v>18937.566436409343</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="D13" s="11">
+        <v>53.567999999999998</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:16" ht="19">
+      <c r="A14" s="7"/>
+      <c r="B14" s="10">
+        <v>1778.961055137132</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="D11" s="16">
-        <v>479.988</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="J11" s="17">
-        <v>12321</v>
-      </c>
-      <c r="K11" s="18"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" ht="19">
-      <c r="A12" s="8"/>
-      <c r="B12" s="15">
-        <v>18446.91754397425</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D12" s="16">
-        <v>11.808</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="20" t="s">
+      <c r="D14" s="11">
+        <v>503.96000000000004</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:16" ht="19">
+      <c r="A15" s="7"/>
+      <c r="B15" s="10">
+        <v>13846.826141617345</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="11">
+        <v>21.34</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+    </row>
+    <row r="16" spans="1:16" ht="19">
+      <c r="A16" s="7"/>
+      <c r="B16" s="10">
+        <v>7812.0517691857222</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="11">
+        <v>36.4</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="1:16" ht="19">
+      <c r="A17" s="7"/>
+      <c r="B17" s="10">
+        <v>10006.670029861949</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" s="11">
+        <v>51.75</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I12" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="J12" s="21">
-        <v>25921</v>
-      </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:17" ht="19">
-      <c r="A13" s="8"/>
-      <c r="B13" s="15">
-        <v>22337.723635387698</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D13" s="16">
-        <v>53.567999999999998</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:17" ht="19">
-      <c r="A14" s="8"/>
-      <c r="B14" s="15">
-        <v>1778.961055137132</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="D14" s="16">
-        <v>503.96000000000004</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:17" ht="19">
-      <c r="A15" s="8"/>
-      <c r="B15" s="15">
-        <v>13846.826141617345</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="D15" s="16">
-        <v>21.34</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:17" ht="19">
-      <c r="A16" s="8"/>
-      <c r="B16" s="15">
-        <v>7812.0517691857222</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D16" s="16">
-        <v>36.4</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16" ht="19">
-      <c r="A17" s="8"/>
-      <c r="B17" s="15">
-        <v>10006.670029861949</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="19">
+      <c r="A18" s="7"/>
+      <c r="B18" s="10">
+        <v>21558.334885316995</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="D17" s="16">
-        <v>51.75</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27" t="s">
+      <c r="D18" s="11">
+        <v>15.51</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="19">
-      <c r="A18" s="8"/>
-      <c r="B18" s="15">
-        <v>21558.334885316995</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="I18" s="8">
+        <v>1</v>
+      </c>
+      <c r="J18" s="8">
+        <v>2</v>
+      </c>
+      <c r="K18" s="8">
+        <v>3</v>
+      </c>
+      <c r="L18" s="8">
+        <v>4</v>
+      </c>
+      <c r="M18" s="8">
+        <v>5</v>
+      </c>
+      <c r="N18" s="8">
+        <v>6</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="1:16" ht="19">
+      <c r="A19" s="7"/>
+      <c r="B19" s="10">
+        <v>16033.292493818983</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="D18" s="16">
-        <v>15.51</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="27" t="s">
+      <c r="D19" s="11">
+        <v>146.82</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8">
+        <v>20</v>
+      </c>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="19">
+      <c r="A20" s="7"/>
+      <c r="B20" s="10">
+        <v>7513.8415119297551</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="11">
+        <v>12.96</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8">
+        <v>40</v>
+      </c>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="19">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8">
+        <v>60</v>
+      </c>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="I18" s="27">
-        <v>1</v>
-      </c>
-      <c r="J18" s="27">
-        <v>2</v>
-      </c>
-      <c r="K18" s="27">
-        <v>3</v>
-      </c>
-      <c r="L18" s="13">
-        <v>4</v>
-      </c>
-      <c r="M18" s="13">
-        <v>5</v>
-      </c>
-      <c r="N18" s="13">
-        <v>6</v>
-      </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="19" spans="1:16" ht="19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="15">
-        <v>16033.292493818983</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="D19" s="16">
-        <v>146.82</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="13">
-        <v>20</v>
-      </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="19" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="19">
-      <c r="A20" s="8"/>
-      <c r="B20" s="15">
-        <v>7513.8415119297551</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="16">
-        <v>12.96</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="13">
-        <v>40</v>
-      </c>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="19" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="19">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="24" t="s">
+    </row>
+    <row r="22" spans="1:16" ht="19">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8">
+        <v>80</v>
+      </c>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="19">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="19" t="s">
+      <c r="D23" s="13"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="13">
-        <v>60</v>
-      </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="19" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="19">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="13">
-        <v>80</v>
-      </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="19" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="19">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="24" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="8">
+        <v>100</v>
+      </c>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+    </row>
+    <row r="24" spans="1:16" ht="19">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8">
+        <v>250</v>
+      </c>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+    </row>
+    <row r="25" spans="1:16" ht="19">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="19" t="s">
+      <c r="D25" s="13"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="13">
-        <v>100</v>
-      </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-    </row>
-    <row r="24" spans="1:16" ht="19">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="13">
-        <v>250</v>
-      </c>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" spans="1:16" ht="19">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="13">
+      <c r="G25" s="7"/>
+      <c r="H25" s="8">
         <v>500</v>
       </c>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
     </row>
     <row r="26" spans="1:16" ht="19">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:16" ht="19">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4533,7 +4446,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{628B8DB5-4744-6946-9D78-7DBDCD361712}">
-  <dimension ref="A3:Q27"/>
+  <dimension ref="B3:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -4546,515 +4459,510 @@
     <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" ht="45" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" ht="19">
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" ht="19">
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" ht="19">
-      <c r="B6" s="10" t="s">
+    <row r="3" spans="2:17" ht="45" customHeight="1">
+      <c r="B3" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="2:17" ht="19">
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+    </row>
+    <row r="5" spans="2:17" ht="19">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="2:17" ht="19">
+      <c r="B6" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="H6" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="L6" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="2:17" ht="19">
+      <c r="B7" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="H6" s="29" t="s">
+      <c r="C7" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="M7" s="11">
+        <v>44</v>
+      </c>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="2:17" ht="19">
+      <c r="B8" s="10">
+        <v>15131.229278417033</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="11">
+        <v>128.05799999999999</v>
+      </c>
+      <c r="H8" s="10">
+        <v>22337.723635387698</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="22"/>
+      <c r="L8" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="M8" s="11">
+        <v>53</v>
+      </c>
+      <c r="N8" s="8">
+        <v>2</v>
+      </c>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="2:17" ht="19">
+      <c r="B9" s="10">
+        <v>21689.879773785746</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" s="11">
+        <v>58.407999999999994</v>
+      </c>
+      <c r="H9" s="10">
+        <v>10006.670029861949</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="22"/>
+      <c r="L9" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="M9" s="11">
+        <v>17</v>
+      </c>
+      <c r="N9" s="8">
+        <v>3</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="2:17" ht="19">
+      <c r="B10" s="10">
+        <v>6556.4431594744028</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D10" s="11">
+        <v>79.97399999999999</v>
+      </c>
+      <c r="H10" s="10">
+        <v>18937.566436409343</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="22"/>
+      <c r="L10" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="M10" s="11">
+        <v>25</v>
+      </c>
+      <c r="N10" s="8">
+        <v>4</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="2:17" ht="19">
+      <c r="B11" s="10">
+        <v>18937.566436409343</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" s="11">
+        <v>479.988</v>
+      </c>
+      <c r="H11" s="10">
+        <v>16033.292493818983</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="22"/>
+      <c r="L11" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="M11" s="11">
+        <v>56</v>
+      </c>
+      <c r="N11" s="8">
+        <v>5</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="2:17" ht="19">
+      <c r="B12" s="10">
+        <v>18446.91754397425</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="11">
+        <v>11.808</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1778.961055137132</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="22"/>
+      <c r="L12" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="M12" s="11">
+        <v>25</v>
+      </c>
+      <c r="N12" s="8">
+        <v>6</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="2:17" ht="19">
+      <c r="B13" s="10">
+        <v>22337.723635387698</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13" s="11">
+        <v>53.567999999999998</v>
+      </c>
+      <c r="H13" s="10">
+        <v>7812.0517691857222</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="22"/>
+      <c r="L13" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="M13" s="11">
+        <v>150</v>
+      </c>
+      <c r="N13" s="8">
+        <v>7</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="2:17" ht="19">
+      <c r="B14" s="10">
+        <v>1778.961055137132</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="11">
+        <v>503.96000000000004</v>
+      </c>
+      <c r="H14" s="10">
+        <v>21558.334885316995</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="22"/>
+      <c r="L14" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="M14" s="11">
+        <v>100</v>
+      </c>
+      <c r="N14" s="8">
+        <v>8</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="2:17" ht="19">
+      <c r="B15" s="10">
+        <v>13846.826141617345</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="11">
+        <v>21.34</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M15" s="11">
+        <v>225</v>
+      </c>
+      <c r="N15" s="8">
+        <v>9</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="2:17" ht="19">
+      <c r="B16" s="10">
+        <v>7812.0517691857222</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="11">
+        <v>36.4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>257</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="M16" s="11">
+        <v>225</v>
+      </c>
+      <c r="N16" s="8">
+        <v>10</v>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="2:17" ht="19">
+      <c r="B17" s="10">
+        <v>10006.670029861949</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" s="11">
+        <v>51.75</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="L6" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="N6" s="14" t="s">
+      <c r="L17" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="M17" s="11">
+        <v>189.55</v>
+      </c>
+      <c r="N17" s="8">
+        <v>11</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="2:17" ht="19">
+      <c r="B18" s="10">
+        <v>21558.334885316995</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18" s="11">
+        <v>15.51</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="M18" s="11">
+        <v>189.55</v>
+      </c>
+      <c r="N18" s="8">
+        <v>12</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="2:17" ht="19">
+      <c r="B19" s="10">
+        <v>16033.292493818983</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="11">
+        <v>146.82</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="2:17" ht="19">
+      <c r="B20" s="10">
+        <v>7513.8415119297551</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="11">
+        <v>12.96</v>
+      </c>
+      <c r="F20" t="s">
+        <v>257</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" ht="19">
-      <c r="B7" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="M7" s="16">
-        <v>44</v>
-      </c>
-      <c r="N7" s="13">
-        <v>1</v>
-      </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-    </row>
-    <row r="8" spans="1:17" ht="19">
-      <c r="B8" s="15">
-        <v>15131.229278417033</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="D8" s="16">
-        <v>128.05799999999999</v>
-      </c>
-      <c r="H8" s="15">
-        <v>22337.723635387698</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="30"/>
-      <c r="L8" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="M8" s="16">
-        <v>53</v>
-      </c>
-      <c r="N8" s="13">
-        <v>2</v>
-      </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-    </row>
-    <row r="9" spans="1:17" ht="19">
-      <c r="B9" s="15">
-        <v>21689.879773785746</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D9" s="16">
-        <v>58.407999999999994</v>
-      </c>
-      <c r="H9" s="15">
-        <v>10006.670029861949</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="30"/>
-      <c r="L9" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="M9" s="16">
-        <v>17</v>
-      </c>
-      <c r="N9" s="13">
-        <v>3</v>
-      </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" ht="19">
-      <c r="B10" s="15">
-        <v>6556.4431594744028</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D10" s="16">
-        <v>79.97399999999999</v>
-      </c>
-      <c r="H10" s="15">
-        <v>18937.566436409343</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="30"/>
-      <c r="L10" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="M10" s="16">
-        <v>25</v>
-      </c>
-      <c r="N10" s="13">
-        <v>4</v>
-      </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" ht="19">
-      <c r="B11" s="15">
-        <v>18937.566436409343</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="D11" s="16">
-        <v>479.988</v>
-      </c>
-      <c r="H11" s="15">
-        <v>16033.292493818983</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="30"/>
-      <c r="L11" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="M11" s="16">
-        <v>56</v>
-      </c>
-      <c r="N11" s="13">
-        <v>5</v>
-      </c>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" ht="19">
-      <c r="B12" s="15">
-        <v>18446.91754397425</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D12" s="16">
-        <v>11.808</v>
-      </c>
-      <c r="H12" s="15">
-        <v>1778.961055137132</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="30"/>
-      <c r="L12" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="M12" s="16">
-        <v>25</v>
-      </c>
-      <c r="N12" s="13">
-        <v>6</v>
-      </c>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-    </row>
-    <row r="13" spans="1:17" ht="19">
-      <c r="B13" s="15">
-        <v>22337.723635387698</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D13" s="16">
-        <v>53.567999999999998</v>
-      </c>
-      <c r="H13" s="15">
-        <v>7812.0517691857222</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="30"/>
-      <c r="L13" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="M13" s="16">
-        <v>150</v>
-      </c>
-      <c r="N13" s="13">
-        <v>7</v>
-      </c>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-    </row>
-    <row r="14" spans="1:17" ht="19">
-      <c r="B14" s="15">
-        <v>1778.961055137132</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="D14" s="16">
-        <v>503.96000000000004</v>
-      </c>
-      <c r="H14" s="15">
-        <v>21558.334885316995</v>
-      </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="30"/>
-      <c r="L14" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="M14" s="16">
-        <v>100</v>
-      </c>
-      <c r="N14" s="13">
-        <v>8</v>
-      </c>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-    </row>
-    <row r="15" spans="1:17" ht="19">
-      <c r="B15" s="15">
-        <v>13846.826141617345</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="D15" s="16">
-        <v>21.34</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="M15" s="16">
-        <v>225</v>
-      </c>
-      <c r="N15" s="13">
-        <v>9</v>
-      </c>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-    </row>
-    <row r="16" spans="1:17" ht="19">
-      <c r="B16" s="15">
-        <v>7812.0517691857222</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D16" s="16">
-        <v>36.4</v>
-      </c>
-      <c r="H16" t="s">
-        <v>258</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="M16" s="16">
-        <v>225</v>
-      </c>
-      <c r="N16" s="13">
-        <v>10</v>
-      </c>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-    </row>
-    <row r="17" spans="2:17" ht="19">
-      <c r="B17" s="15">
-        <v>10006.670029861949</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D17" s="16">
-        <v>51.75</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="M17" s="16">
-        <v>189.55</v>
-      </c>
-      <c r="N17" s="13">
-        <v>11</v>
-      </c>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-    </row>
-    <row r="18" spans="2:17" ht="19">
-      <c r="B18" s="15">
-        <v>21558.334885316995</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="D18" s="16">
-        <v>15.51</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="M18" s="16">
-        <v>189.55</v>
-      </c>
-      <c r="N18" s="13">
-        <v>12</v>
-      </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-    </row>
-    <row r="19" spans="2:17" ht="19">
-      <c r="B19" s="15">
-        <v>16033.292493818983</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="D19" s="16">
-        <v>146.82</v>
-      </c>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-    </row>
-    <row r="20" spans="2:17" ht="19">
-      <c r="B20" s="15">
-        <v>7513.8415119297551</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="16">
-        <v>12.96</v>
-      </c>
-      <c r="F20" t="s">
-        <v>258</v>
-      </c>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="24" t="s">
+      <c r="O20" s="13"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="2:17" ht="19">
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="2:17" ht="19">
+      <c r="C22" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="2:17" ht="19">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="20"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="O20" s="18"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-    </row>
-    <row r="21" spans="2:17" ht="19">
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-    </row>
-    <row r="22" spans="2:17" ht="19">
-      <c r="C22" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="19" t="s">
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="24" spans="2:17" ht="19">
+      <c r="C24" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q22" s="8"/>
-    </row>
-    <row r="23" spans="2:17" ht="19">
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="25"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="19" t="s">
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="Q23" s="8"/>
-    </row>
-    <row r="24" spans="2:17" ht="19">
-      <c r="C24" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="19" t="s">
-        <v>283</v>
-      </c>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q24" s="8"/>
+      <c r="Q24" s="7"/>
     </row>
     <row r="25" spans="2:17" ht="19">
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
     </row>
     <row r="26" spans="2:17" ht="19">
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
     </row>
     <row r="27" spans="2:17" ht="19">
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>